<commit_message>
2025 roswell data added
</commit_message>
<xml_diff>
--- a/Drug lists/BetaBlockerDrugNames.xlsx
+++ b/Drug lists/BetaBlockerDrugNames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD work\clinpath_CT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD work\clinpath_CT\Drug lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799088E-5C3D-45AC-873F-94345AC1770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E833448B-7CCC-4B59-A317-ACB3117E0598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{81B96F5C-5FD5-ED4A-A5B6-FDD91649B013}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{81B96F5C-5FD5-ED4A-A5B6-FDD91649B013}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
   <si>
     <t>acebutolol hydrochloride</t>
   </si>
@@ -1240,6 +1240,15 @@
   </si>
   <si>
     <t>Mepindolol</t>
+  </si>
+  <si>
+    <t>toprol-xl</t>
+  </si>
+  <si>
+    <t>atenolol</t>
+  </si>
+  <si>
+    <t>metoprol</t>
   </si>
 </sst>
 </file>
@@ -1275,9 +1284,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1603,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42888611-9803-1B4B-9CFB-C4EEB3CF7192}">
-  <dimension ref="A1:A402"/>
+  <dimension ref="A1:A405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
+      <selection activeCell="A406" sqref="A406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1755,7 +1763,7 @@
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>400</v>
       </c>
     </row>
@@ -3622,6 +3630,21 @@
     <row r="402" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A403" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A404" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A405" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>